<commit_message>
edit Evaluasi Wireframe Aplikasi CompleX (Jawaban).xlsx
</commit_message>
<xml_diff>
--- a/Evaluasi/data/Evaluasi Wireframe Aplikasi CompleX (Jawaban).xlsx
+++ b/Evaluasi/data/Evaluasi Wireframe Aplikasi CompleX (Jawaban).xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New Volume D\S4\Interaksi Manusia &amp; Komputer\Tugas\CyberRom\REVISI\EVALUASI\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4559C73D-6FFB-4D84-B559-7AA0FC411070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -154,18 +163,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -176,11 +186,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="13">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF442F65"/>
@@ -194,6 +210,7 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -208,6 +225,7 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -222,6 +240,7 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -236,6 +255,7 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -250,6 +270,7 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -264,6 +285,7 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -278,6 +300,7 @@
       <bottom style="thin">
         <color rgb="FFF8F9FA"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -292,6 +315,7 @@
       <bottom style="thin">
         <color rgb="FFF8F9FA"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -306,6 +330,7 @@
       <bottom style="thin">
         <color rgb="FFF8F9FA"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -320,6 +345,7 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -334,6 +360,7 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -348,153 +375,1353 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8F9FA"/>
+          <bgColor rgb="FFF8F9FA"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF5B3F86"/>
           <bgColor rgb="FF5B3F86"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8F9FA"/>
-          <bgColor rgb="FFF8F9FA"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="Form Responses 1-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    <tableStyle name="Form Responses 1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>248478</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>39456</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>590833</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>177195</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Diagram jawaban Formulir. Judul pertanyaan: Apa peran anda. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CE54A1B-01E9-D3B8-F5FD-2839765354D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="248478" y="1828499"/>
+          <a:ext cx="4119225" cy="1728000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>248478</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>53106</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>624333</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>190845</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Diagram jawaban Formulir. Judul pertanyaan: Rentang umur anda. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0792B19-411C-923C-1071-E398C07FDC95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="248478" y="3631193"/>
+          <a:ext cx="4152725" cy="1728000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>705975</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>198782</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1902274</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>67304</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="Diagram jawaban Formulir. Judul pertanyaan: Berdasarkan wireframe, saya merasa akan mudah melihat status tindakan saya, seperti apakah laporan saya sedang diproses (misalnya, ada indikator loading atau konfirmasi).. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{118C715E-665C-0EB7-BE81-2842F1B23D28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4482845" y="1789043"/>
+          <a:ext cx="2504951" cy="1260000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>720586</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>165652</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1899778</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>34174</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="Diagram jawaban Formulir. Judul pertanyaan: Ikon dan istilah yang ditampilkan di wireframe (misalnya, ikon &quot;Tombol Panik&quot; atau &quot;Laporkan Kebersihan&quot;) terlihat mudah dipahami dan sesuai dengan bahasa sehari-hari saya.. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70707F87-CCE4-1028-80AF-439A44E3A97E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4497456" y="3147391"/>
+          <a:ext cx="2487844" cy="1260000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>728869</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>132522</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1908061</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1043</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="Diagram jawaban Formulir. Judul pertanyaan: Berdasarkan wireframe, saya merasa akan mudah membatalkan atau kembali dari suatu tindakan (misalnya, keluar dari formulir laporan tanpa mengirim).. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D33C096-A548-4A76-7F04-40B9853CDE6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4505739" y="4505739"/>
+          <a:ext cx="2487844" cy="1260000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>745434</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>26504</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1924626</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>93809</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="Diagram jawaban Formulir. Judul pertanyaan: Wireframe menunjukkan desain yang konsisten di setiap layar (misalnya, ikon dan tata letak tombol terlihat seragam di halaman login dan halaman utama).. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61D2245C-5D3A-FDDF-F377-9CFDF9DBF5DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4522304" y="5791200"/>
+          <a:ext cx="2487844" cy="1260000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>745434</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>191329</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1924626</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>59850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="Diagram jawaban Formulir. Judul pertanyaan: Wireframe terlihat mendukung pencegahan kesalahan (misalnya, ada tanda kolom wajib di formulir laporan sehingga saya tidak salah mengisi).. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{425F137B-20C8-CADA-4F62-BC6C013E79BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4522304" y="7148720"/>
+          <a:ext cx="2487844" cy="1260000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>745434</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>157369</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1924626</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>25891</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="Diagram jawaban Formulir. Judul pertanyaan: Berdasarkan wireframe, saya merasa dapat mengenali fungsi tombol atau ikon dengan mudah tanpa harus mengingat (misalnya, ikon &quot;Beranda&quot; atau &quot;Tombol Panik&quot; terlihat jelas).. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84C950B7-4B25-C36A-3DCE-F9AE1041BAC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4522304" y="8506239"/>
+          <a:ext cx="2487844" cy="1260000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2345225</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>128379</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2331721</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>195683</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10" descr="Diagram jawaban Formulir. Judul pertanyaan: Wireframe terlihat memungkinkan saya menyelesaikan tugas dengan efisien, baik sebagai pengguna baru maupun berpengalaman (misalnya, akses cepat ke fitur laporan untuk satpam, atau navigasi mudah untuk warga).. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B96032A1-21C6-61BD-ED87-52CD51DA1686}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7430747" y="1718640"/>
+          <a:ext cx="2487844" cy="1260000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2345225</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>142460</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2331721</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>10982</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11" descr="Diagram jawaban Formulir. Judul pertanyaan: Tampilan wireframe terlihat bersih dan hanya menampilkan elemen yang relevan tanpa ada bagian yang terasa berlebihan (misalnya, layar utama tidak terlalu penuh).. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{884EEF0A-F328-1594-4502-BA08D945012B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7430747" y="3124199"/>
+          <a:ext cx="2487844" cy="1260000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>745434</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>128379</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1941733</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>195683</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12" descr="Diagram jawaban Formulir. Judul pertanyaan: Berdasarkan wireframe, saya merasa akan mudah melihat status tindakan saya, seperti apakah laporan saya sedang diproses (misalnya, ada indikator loading atau konfirmasi).. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C4520BB-6912-1E6C-D51C-89166A24F18A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4522304" y="1718640"/>
+          <a:ext cx="2504951" cy="1260000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>745434</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>94421</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1924626</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13" descr="Diagram jawaban Formulir. Judul pertanyaan: Ikon dan istilah yang ditampilkan di wireframe (misalnya, ikon &quot;Tombol Panik&quot; atau &quot;Laporkan Kebersihan&quot;) terlihat mudah dipahami dan sesuai dengan bahasa sehari-hari saya.. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C301D08-F14B-4033-8525-ED2BD402BB42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4522304" y="3076160"/>
+          <a:ext cx="2487844" cy="1260000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>745434</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>60463</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1924626</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>127767</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14" descr="Diagram jawaban Formulir. Judul pertanyaan: Berdasarkan wireframe, saya merasa akan mudah membatalkan atau kembali dari suatu tindakan (misalnya, keluar dari formulir laporan tanpa mengirim).. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDC5111C-F3B7-5059-088A-A61C23C83D70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4522304" y="4433680"/>
+          <a:ext cx="2487844" cy="1260000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2345225</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>156541</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2331721</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>25062</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15" descr="Diagram jawaban Formulir. Judul pertanyaan: Berdasarkan wireframe, saya merasa pesan kesalahan (misalnya, saat gagal login) akan ditampilkan dengan jelas dan membantu saya memahami cara memperbaikinya.. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7047A187-5229-84A7-1B9F-5EC8248EA735}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7430747" y="4529758"/>
+          <a:ext cx="2487844" cy="1260000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2345225</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>170621</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2331721</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>39143</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16" descr="Diagram jawaban Formulir. Judul pertanyaan: Wireframe menunjukkan adanya fitur bantuan yang mudah diakses (misalnya, ikon bantuan atau panduan untuk fitur seperti pelaporan).. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E8986BE-EF9A-9504-E442-7F75A21AC827}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7430747" y="5935317"/>
+          <a:ext cx="2487844" cy="1260000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2345225</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>184702</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2331721</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>53224</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17" descr="Diagram jawaban Formulir. Judul pertanyaan: Seberapa mudah menemukan fitur &quot;Tombol Panik&quot; untuk keadaan darurat berdasarkan tata letak wireframe?. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C969EA7F-386B-E8DF-74FB-CF33032DD60E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7430747" y="7340876"/>
+          <a:ext cx="2487844" cy="1260000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2345225</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2331721</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>67305</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18" descr="Diagram jawaban Formulir. Judul pertanyaan: Berdasarkan wireframe, seberapa jelas langkah-langkah untuk mengirim laporan kebersihan atau keamanan (misalnya, tata letak formulir laporan)?. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57BA0841-597F-1DFE-A8EA-177DD3D79DBC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7430747" y="8746435"/>
+          <a:ext cx="2487844" cy="1260000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>223630</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>128379</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>210126</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>195683</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19" descr="Diagram jawaban Formulir. Judul pertanyaan: Seberapa jelas bilah navigasi di bagian bawah wireframe untuk mengakses fitur berbeda (misalnya, beranda, laporan, profil)?. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1905110-3D56-96E7-9217-8DAD0E55BCAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10311847" y="1718640"/>
+          <a:ext cx="2487844" cy="1260000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>223629</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>190498</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1141286</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>21454</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20" descr="Diagram jawaban Formulir. Judul pertanyaan: Apa yang paling Anda sukai dari desain wireframe aplikasi CompleX?. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98B7B390-ED99-90AA-F85E-1EBAB0A43702}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10311846" y="3172237"/>
+          <a:ext cx="3419005" cy="1620000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>223629</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>124238</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1306176</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>153978</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21" descr="Diagram jawaban Formulir. Judul pertanyaan: Berdasarkan wireframe ini, apakah Anda merasa akan menggunakan aplikasi CompleX untuk mengelola keamanan, kebersihan, atau reservasi fasilitas di komplek Anda?. Jumlah jawaban: 7 jawaban.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AC05421-CF9B-26F6-BF03-5132A7E58370}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10311846" y="4895021"/>
+          <a:ext cx="3583895" cy="1620000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:T8" displayName="Form_Responses1" name="Form_Responses1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:T8">
   <tableColumns count="20">
-    <tableColumn name="Timestamp" id="1"/>
-    <tableColumn name="Email Address" id="2"/>
-    <tableColumn name="Apa peran anda" id="3"/>
-    <tableColumn name="Rentang umur anda" id="4"/>
-    <tableColumn name="Berdasarkan wireframe, saya merasa akan mudah melihat status tindakan saya, seperti apakah laporan saya sedang diproses (misalnya, ada indikator loading atau konfirmasi)." id="5"/>
-    <tableColumn name="Ikon dan istilah yang ditampilkan di wireframe (misalnya, ikon &quot;Tombol Panik&quot; atau &quot;Laporkan Kebersihan&quot;) terlihat mudah dipahami dan sesuai dengan bahasa sehari-hari saya." id="6"/>
-    <tableColumn name="Berdasarkan wireframe, saya merasa akan mudah membatalkan atau kembali dari suatu tindakan (misalnya, keluar dari formulir laporan tanpa mengirim)." id="7"/>
-    <tableColumn name="Wireframe menunjukkan desain yang konsisten di setiap layar (misalnya, ikon dan tata letak tombol terlihat seragam di halaman login dan halaman utama)." id="8"/>
-    <tableColumn name="Wireframe terlihat mendukung pencegahan kesalahan (misalnya, ada tanda kolom wajib di formulir laporan sehingga saya tidak salah mengisi)." id="9"/>
-    <tableColumn name="Berdasarkan wireframe, saya merasa dapat mengenali fungsi tombol atau ikon dengan mudah tanpa harus mengingat (misalnya, ikon &quot;Beranda&quot; atau &quot;Tombol Panik&quot; terlihat jelas)." id="10"/>
-    <tableColumn name="Wireframe terlihat memungkinkan saya menyelesaikan tugas dengan efisien, baik sebagai pengguna baru maupun berpengalaman (misalnya, akses cepat ke fitur laporan untuk satpam, atau navigasi mudah untuk warga)." id="11"/>
-    <tableColumn name="Tampilan wireframe terlihat bersih dan hanya menampilkan elemen yang relevan tanpa ada bagian yang terasa berlebihan (misalnya, layar utama tidak terlalu penuh)." id="12"/>
-    <tableColumn name="Berdasarkan wireframe, saya merasa pesan kesalahan (misalnya, saat gagal login) akan ditampilkan dengan jelas dan membantu saya memahami cara memperbaikinya." id="13"/>
-    <tableColumn name="Wireframe menunjukkan adanya fitur bantuan yang mudah diakses (misalnya, ikon bantuan atau panduan untuk fitur seperti pelaporan)." id="14"/>
-    <tableColumn name="Seberapa mudah menemukan fitur &quot;Tombol Panik&quot; untuk keadaan darurat berdasarkan tata letak wireframe?" id="15"/>
-    <tableColumn name="Berdasarkan wireframe, seberapa jelas langkah-langkah untuk mengirim laporan kebersihan atau keamanan (misalnya, tata letak formulir laporan)?" id="16"/>
-    <tableColumn name="Seberapa jelas bilah navigasi di bagian bawah wireframe untuk mengakses fitur berbeda (misalnya, beranda, laporan, profil)?" id="17"/>
-    <tableColumn name="Apa yang paling Anda sukai dari desain wireframe aplikasi CompleX?" id="18"/>
-    <tableColumn name="Apa saran perbaikan Anda untuk desain wireframe aplikasi CompleX?" id="19"/>
-    <tableColumn name="Berdasarkan wireframe ini, apakah Anda merasa akan menggunakan aplikasi CompleX untuk mengelola keamanan, kebersihan, atau reservasi fasilitas di komplek Anda?" id="20"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Timestamp"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Email Address"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Apa peran anda"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Rentang umur anda"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Berdasarkan wireframe, saya merasa akan mudah melihat status tindakan saya, seperti apakah laporan saya sedang diproses (misalnya, ada indikator loading atau konfirmasi)."/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Ikon dan istilah yang ditampilkan di wireframe (misalnya, ikon &quot;Tombol Panik&quot; atau &quot;Laporkan Kebersihan&quot;) terlihat mudah dipahami dan sesuai dengan bahasa sehari-hari saya."/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Berdasarkan wireframe, saya merasa akan mudah membatalkan atau kembali dari suatu tindakan (misalnya, keluar dari formulir laporan tanpa mengirim)."/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Wireframe menunjukkan desain yang konsisten di setiap layar (misalnya, ikon dan tata letak tombol terlihat seragam di halaman login dan halaman utama)."/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Wireframe terlihat mendukung pencegahan kesalahan (misalnya, ada tanda kolom wajib di formulir laporan sehingga saya tidak salah mengisi)."/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Berdasarkan wireframe, saya merasa dapat mengenali fungsi tombol atau ikon dengan mudah tanpa harus mengingat (misalnya, ikon &quot;Beranda&quot; atau &quot;Tombol Panik&quot; terlihat jelas)."/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Wireframe terlihat memungkinkan saya menyelesaikan tugas dengan efisien, baik sebagai pengguna baru maupun berpengalaman (misalnya, akses cepat ke fitur laporan untuk satpam, atau navigasi mudah untuk warga)."/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tampilan wireframe terlihat bersih dan hanya menampilkan elemen yang relevan tanpa ada bagian yang terasa berlebihan (misalnya, layar utama tidak terlalu penuh)."/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Berdasarkan wireframe, saya merasa pesan kesalahan (misalnya, saat gagal login) akan ditampilkan dengan jelas dan membantu saya memahami cara memperbaikinya."/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Wireframe menunjukkan adanya fitur bantuan yang mudah diakses (misalnya, ikon bantuan atau panduan untuk fitur seperti pelaporan)."/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Seberapa mudah menemukan fitur &quot;Tombol Panik&quot; untuk keadaan darurat berdasarkan tata letak wireframe?"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Berdasarkan wireframe, seberapa jelas langkah-langkah untuk mengirim laporan kebersihan atau keamanan (misalnya, tata letak formulir laporan)?"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Seberapa jelas bilah navigasi di bagian bawah wireframe untuk mengakses fitur berbeda (misalnya, beranda, laporan, profil)?"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Apa yang paling Anda sukai dari desain wireframe aplikasi CompleX?"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Apa saran perbaikan Anda untuk desain wireframe aplikasi CompleX?"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Berdasarkan wireframe ini, apakah Anda merasa akan menggunakan aplikasi CompleX untuk mengelola keamanan, kebersihan, atau reservasi fasilitas di komplek Anda?"/>
   </tableColumns>
-  <tableStyleInfo name="Form Responses 1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Form Responses 1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -684,29 +1911,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="3" width="18.88"/>
-    <col customWidth="1" min="4" max="4" width="19.63"/>
-    <col customWidth="1" min="5" max="20" width="37.63"/>
-    <col customWidth="1" min="21" max="26" width="18.88"/>
+    <col min="1" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="20" width="37.5703125" customWidth="1"/>
+    <col min="21" max="26" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -768,7 +1998,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>45787.77355677083</v>
       </c>
@@ -782,43 +2012,43 @@
         <v>22</v>
       </c>
       <c r="E2" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F2" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="G2" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H2" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I2" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="J2" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="K2" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L2" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M2" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="N2" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="O2" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="P2" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="Q2" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>23</v>
@@ -830,7 +2060,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>45787.776332696754</v>
       </c>
@@ -844,53 +2074,53 @@
         <v>22</v>
       </c>
       <c r="E3" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F3" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="G3" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H3" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I3" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="J3" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="K3" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L3" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="M3" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="N3" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="O3" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="P3" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q3" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="R3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="S3" s="9"/>
-      <c r="T3" s="10" t="s">
+      <c r="S3" s="8"/>
+      <c r="T3" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>45787.77805552083</v>
       </c>
@@ -904,43 +2134,43 @@
         <v>22</v>
       </c>
       <c r="E4" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F4" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="G4" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H4" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I4" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="J4" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="K4" s="5">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L4" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M4" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="N4" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="O4" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="P4" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="Q4" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>30</v>
@@ -952,9 +2182,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
-        <v>45787.78530239583</v>
+        <v>45787.785302395831</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>33</v>
@@ -966,43 +2196,43 @@
         <v>22</v>
       </c>
       <c r="E5" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="F5" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="G5" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="H5" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="I5" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J5" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="K5" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L5" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="M5" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="N5" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="O5" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="P5" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="Q5" s="8">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>34</v>
@@ -1010,13 +2240,13 @@
       <c r="S5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="T5" s="10" t="s">
+      <c r="T5" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>45787.7906442824</v>
+        <v>45787.790644282402</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>36</v>
@@ -1028,180 +2258,181 @@
         <v>22</v>
       </c>
       <c r="E6" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F6" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="G6" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H6" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="I6" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="J6" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="K6" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L6" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M6" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="N6" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="O6" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="P6" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="Q6" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="S6" s="11"/>
+      <c r="S6" s="5"/>
       <c r="T6" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="12">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
         <v>45787.824628055554</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="F7" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="G7" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="H7" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="I7" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="J7" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="K7" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="L7" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="M7" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="N7" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="O7" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="P7" s="13">
-        <v>4.0</v>
-      </c>
-      <c r="Q7" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="R7" s="13" t="s">
+      <c r="E7" s="8">
+        <v>5</v>
+      </c>
+      <c r="F7" s="8">
+        <v>5</v>
+      </c>
+      <c r="G7" s="8">
+        <v>5</v>
+      </c>
+      <c r="H7" s="8">
+        <v>5</v>
+      </c>
+      <c r="I7" s="8">
+        <v>5</v>
+      </c>
+      <c r="J7" s="8">
+        <v>5</v>
+      </c>
+      <c r="K7" s="8">
+        <v>5</v>
+      </c>
+      <c r="L7" s="8">
+        <v>5</v>
+      </c>
+      <c r="M7" s="8">
+        <v>5</v>
+      </c>
+      <c r="N7" s="8">
+        <v>5</v>
+      </c>
+      <c r="O7" s="8">
+        <v>5</v>
+      </c>
+      <c r="P7" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>5</v>
+      </c>
+      <c r="R7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="S7" s="13" t="s">
+      <c r="S7" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="T7" s="14" t="s">
+      <c r="T7" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="15">
-        <v>45787.94097322917</v>
-      </c>
-      <c r="B8" s="16" t="s">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
+        <v>45787.940973229168</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="16">
-        <v>3.0</v>
-      </c>
-      <c r="F8" s="16">
-        <v>4.0</v>
-      </c>
-      <c r="G8" s="16">
-        <v>3.0</v>
-      </c>
-      <c r="H8" s="16">
-        <v>3.0</v>
-      </c>
-      <c r="I8" s="16">
-        <v>5.0</v>
-      </c>
-      <c r="J8" s="16">
-        <v>3.0</v>
-      </c>
-      <c r="K8" s="16">
-        <v>3.0</v>
-      </c>
-      <c r="L8" s="16">
-        <v>3.0</v>
-      </c>
-      <c r="M8" s="16">
-        <v>5.0</v>
-      </c>
-      <c r="N8" s="16">
-        <v>3.0</v>
-      </c>
-      <c r="O8" s="16">
-        <v>5.0</v>
-      </c>
-      <c r="P8" s="16">
-        <v>5.0</v>
-      </c>
-      <c r="Q8" s="16">
-        <v>3.0</v>
-      </c>
-      <c r="R8" s="16" t="s">
+      <c r="E8" s="11">
+        <v>3</v>
+      </c>
+      <c r="F8" s="11">
+        <v>4</v>
+      </c>
+      <c r="G8" s="11">
+        <v>3</v>
+      </c>
+      <c r="H8" s="11">
+        <v>3</v>
+      </c>
+      <c r="I8" s="11">
+        <v>5</v>
+      </c>
+      <c r="J8" s="11">
+        <v>3</v>
+      </c>
+      <c r="K8" s="11">
+        <v>3</v>
+      </c>
+      <c r="L8" s="11">
+        <v>3</v>
+      </c>
+      <c r="M8" s="11">
+        <v>5</v>
+      </c>
+      <c r="N8" s="11">
+        <v>3</v>
+      </c>
+      <c r="O8" s="11">
+        <v>5</v>
+      </c>
+      <c r="P8" s="11">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="11">
+        <v>3</v>
+      </c>
+      <c r="R8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="S8" s="16" t="s">
+      <c r="S8" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="T8" s="17" t="s">
+      <c r="T8" s="12" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>